<commit_message>
Adicionando mudanças para a apresentacao
</commit_message>
<xml_diff>
--- a/docs/Bancos Relacionais - AlugueAqui/AlugueAqui-logica-2.0.xlsx
+++ b/docs/Bancos Relacionais - AlugueAqui/AlugueAqui-logica-2.0.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Usuario" sheetId="1" r:id="rId1"/>
     <sheet name="Equipamento" sheetId="2" r:id="rId2"/>
     <sheet name="Carrinho" sheetId="3" r:id="rId3"/>
+    <sheet name="ItemCarrinho" sheetId="5" r:id="rId4"/>
+    <sheet name="pedido-aluguel" sheetId="4" r:id="rId5"/>
+    <sheet name="Pagamento" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>Tabela Logica AlugueAqui</t>
   </si>
@@ -183,13 +186,34 @@
   </si>
   <si>
     <t>Carrinho</t>
+  </si>
+  <si>
+    <t>Pedido/Aluguel</t>
+  </si>
+  <si>
+    <t>idPagamento</t>
+  </si>
+  <si>
+    <t>pedido do aluguel</t>
+  </si>
+  <si>
+    <t>ItemCarrinho</t>
+  </si>
+  <si>
+    <t>idEquipamento</t>
+  </si>
+  <si>
+    <t>idPedido/Aluguel</t>
+  </si>
+  <si>
+    <t>Pagamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +240,14 @@
     <font>
       <b/>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -325,8 +357,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,24 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,159 +690,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -836,170 +869,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1017,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1027,60 +1060,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1091,4 +1124,251 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A7:C11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>